<commit_message>
Nov 24 - Updates 1. Updated size reference image to using Eric's monitor and image confidence level 2. Added select_pfolder() per Chetan's request 3. Add a mouse position tool just for dev 4. Added review warning after all BOM fields have been auto-selected 5. Added 1s to open_BOM() time due to delays seen through repeat testing today 6. Modified the screen location coordinates based on Gerber PT 1 default view and various drysuit test trials 7. Removed wait times between data entries in BOM
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhudkins\PycharmProjects\Pattern Automation Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pzou\PycharmProjects\JAX-Efficiency\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029BAB5A-6CA3-47CD-AF4D-DB124226C093}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FCC2DD-337C-4ED4-B458-24994AC1495C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4395" yWindow="30" windowWidth="21600" windowHeight="14685" xr2:uid="{1BEB3B0E-F0ED-4D54-A2F8-1FF6A0E34FB7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1BEB3B0E-F0ED-4D54-A2F8-1FF6A0E34FB7}"/>
   </bookViews>
   <sheets>
     <sheet name="636vNull qty" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3973" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3973" uniqueCount="96">
   <si>
     <t>If requestor is pattern tech, please fill this page.</t>
   </si>
@@ -352,12 +352,15 @@
   <si>
     <t>MSD636G2S-R2</t>
   </si>
+  <si>
+    <t>MSD624G2RSC-R0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,6 +400,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -831,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F3899B6-1DC5-4B97-8067-4625AF99EBA2}">
   <dimension ref="A1:Q928"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5779,7 +5788,7 @@
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B102" t="s">
         <v>23</v>
@@ -5788,12 +5797,11 @@
         <v>59</v>
       </c>
       <c r="D102">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>689</v>
+        <v>100</v>
       </c>
       <c r="E102">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G102" t="s">
         <v>21</v>
@@ -5829,7 +5837,7 @@
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B103" t="s">
         <v>25</v>
@@ -5838,12 +5846,11 @@
         <v>59</v>
       </c>
       <c r="D103">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>731</v>
+        <v>200</v>
       </c>
       <c r="E103">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G103" t="s">
         <v>21</v>
@@ -5879,7 +5886,7 @@
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B104" t="s">
         <v>26</v>
@@ -5888,12 +5895,11 @@
         <v>59</v>
       </c>
       <c r="D104">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>775</v>
+        <v>300</v>
       </c>
       <c r="E104">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H104" t="s">
         <v>48</v>
@@ -5922,7 +5928,7 @@
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B105" t="s">
         <v>27</v>
@@ -5931,12 +5937,11 @@
         <v>59</v>
       </c>
       <c r="D105">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>826</v>
+        <v>400</v>
       </c>
       <c r="E105">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G105" t="s">
         <v>21</v>
@@ -5972,7 +5977,7 @@
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B106" t="s">
         <v>28</v>
@@ -5981,12 +5986,11 @@
         <v>59</v>
       </c>
       <c r="D106">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>867</v>
+        <v>500</v>
       </c>
       <c r="E106">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G106" t="s">
         <v>21</v>
@@ -6022,7 +6026,7 @@
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B107" t="s">
         <v>29</v>
@@ -6031,12 +6035,11 @@
         <v>59</v>
       </c>
       <c r="D107">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>901</v>
+        <v>600</v>
       </c>
       <c r="E107">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G107" t="s">
         <v>21</v>
@@ -6072,7 +6075,7 @@
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B108" t="s">
         <v>30</v>
@@ -6081,12 +6084,11 @@
         <v>59</v>
       </c>
       <c r="D108">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>975</v>
+        <v>700</v>
       </c>
       <c r="E108">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G108" t="s">
         <v>21</v>
@@ -6122,7 +6124,7 @@
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B109" t="s">
         <v>31</v>
@@ -6131,12 +6133,11 @@
         <v>59</v>
       </c>
       <c r="D109">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>1052</v>
+        <v>800</v>
       </c>
       <c r="E109">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G109" t="s">
         <v>21</v>
@@ -6172,7 +6173,7 @@
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B110" t="s">
         <v>32</v>
@@ -6181,12 +6182,11 @@
         <v>59</v>
       </c>
       <c r="D110">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>707</v>
+        <v>900</v>
       </c>
       <c r="E110">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G110" t="s">
         <v>21</v>
@@ -6222,7 +6222,7 @@
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B111" t="s">
         <v>33</v>
@@ -6231,12 +6231,11 @@
         <v>59</v>
       </c>
       <c r="D111">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>749</v>
+        <v>1000</v>
       </c>
       <c r="E111">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G111" t="s">
         <v>21</v>
@@ -6272,7 +6271,7 @@
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B112" t="s">
         <v>34</v>
@@ -6281,12 +6280,11 @@
         <v>59</v>
       </c>
       <c r="D112">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>792</v>
+        <v>1100</v>
       </c>
       <c r="E112">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G112" t="s">
         <v>21</v>
@@ -6321,8 +6319,8 @@
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A113" s="8" t="s">
-        <v>58</v>
+      <c r="A113" t="s">
+        <v>95</v>
       </c>
       <c r="B113" s="8" t="s">
         <v>35</v>
@@ -6331,12 +6329,11 @@
         <v>59</v>
       </c>
       <c r="D113" s="8">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>843</v>
+        <v>1200</v>
       </c>
       <c r="E113">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G113" t="s">
         <v>21</v>
@@ -6372,7 +6369,7 @@
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B114" t="s">
         <v>36</v>
@@ -6381,12 +6378,11 @@
         <v>59</v>
       </c>
       <c r="D114">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>885</v>
+        <v>1300</v>
       </c>
       <c r="E114">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G114" t="s">
         <v>21</v>
@@ -6422,7 +6418,7 @@
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B115" t="s">
         <v>37</v>
@@ -6431,12 +6427,11 @@
         <v>59</v>
       </c>
       <c r="D115">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>919</v>
+        <v>1400</v>
       </c>
       <c r="E115">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G115" t="s">
         <v>21</v>
@@ -6472,7 +6467,7 @@
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B116" t="s">
         <v>38</v>
@@ -6481,12 +6476,11 @@
         <v>59</v>
       </c>
       <c r="D116">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>994</v>
+        <v>1500</v>
       </c>
       <c r="E116">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G116" t="s">
         <v>21</v>
@@ -6522,7 +6516,7 @@
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B117" t="s">
         <v>39</v>
@@ -6531,12 +6525,11 @@
         <v>59</v>
       </c>
       <c r="D117">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>1072</v>
+        <v>1600</v>
       </c>
       <c r="E117">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G117" t="s">
         <v>21</v>
@@ -6572,7 +6565,7 @@
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B118" t="s">
         <v>40</v>
@@ -6581,12 +6574,11 @@
         <v>59</v>
       </c>
       <c r="D118">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>719</v>
+        <v>1700</v>
       </c>
       <c r="E118">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G118" t="s">
         <v>21</v>
@@ -6622,7 +6614,7 @@
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B119" t="s">
         <v>41</v>
@@ -6631,12 +6623,11 @@
         <v>59</v>
       </c>
       <c r="D119">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>762</v>
+        <v>1800</v>
       </c>
       <c r="E119">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G119" t="s">
         <v>21</v>
@@ -6672,7 +6663,7 @@
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B120" t="s">
         <v>42</v>
@@ -6681,12 +6672,11 @@
         <v>59</v>
       </c>
       <c r="D120">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>807</v>
+        <v>1900</v>
       </c>
       <c r="E120">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G120" t="s">
         <v>21</v>
@@ -6722,7 +6712,7 @@
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B121" t="s">
         <v>43</v>
@@ -6731,12 +6721,11 @@
         <v>59</v>
       </c>
       <c r="D121">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>859</v>
+        <v>2000</v>
       </c>
       <c r="E121">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G121" t="s">
         <v>21</v>
@@ -6772,7 +6761,7 @@
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B122" t="s">
         <v>44</v>
@@ -6781,12 +6770,11 @@
         <v>59</v>
       </c>
       <c r="D122">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>901</v>
+        <v>2100</v>
       </c>
       <c r="E122">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G122" t="s">
         <v>21</v>
@@ -6822,7 +6810,7 @@
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B123" t="s">
         <v>45</v>
@@ -6831,12 +6819,11 @@
         <v>59</v>
       </c>
       <c r="D123">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>936</v>
+        <v>2200</v>
       </c>
       <c r="E123">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G123" t="s">
         <v>21</v>
@@ -6872,7 +6859,7 @@
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B124" t="s">
         <v>46</v>
@@ -6881,12 +6868,11 @@
         <v>59</v>
       </c>
       <c r="D124">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>1012</v>
+        <v>2300</v>
       </c>
       <c r="E124">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G124" t="s">
         <v>21</v>
@@ -6922,7 +6908,7 @@
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B125" t="s">
         <v>47</v>
@@ -6931,12 +6917,11 @@
         <v>59</v>
       </c>
       <c r="D125">
-        <f>ROUNDUP(SUMIFS(Table1381114[Total Area],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]]),0)</f>
-        <v>1092</v>
+        <v>2400</v>
       </c>
       <c r="E125">
         <f>SUMIFS(Table1381114['#PCS],Table1381114[MODEL],Table3691215[[#This Row],[MODEL]],Table1381114[SIZES],Table3691215[[#This Row],[SIZES]],Table1381114[FABRIC],Table3691215[[#This Row],[FABRIC]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G125" t="s">
         <v>21</v>
@@ -32859,6 +32844,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="2">

</xml_diff>